<commit_message>
Update FunctionDetailList.xlsx and QAList.xlsx
</commit_message>
<xml_diff>
--- a/BA/QAList.xlsx
+++ b/BA/QAList.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Things\Books\Year 4\Term 1\Capstone\IER PROJECT\branches\htaphuong-prototype\BA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Question</t>
   </si>
@@ -55,6 +60,27 @@
   </si>
   <si>
     <t>Địa chỉ?</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Có cần lưu lịch sử người dùng?</t>
+  </si>
+  <si>
+    <t>Phần "KH mẫu" do khách hàng nhập có nên được ghi vào phần "Ghi chú", sau khi xuất nếu muốn xuất "KH mẫu" theo ý của khách hàng thì cho edit phần đó?</t>
+  </si>
+  <si>
+    <t>Mỗi hành động edit/delete có thể được thực hiện bởi ai và quyền hạn của từng user là như thế nào?</t>
+  </si>
+  <si>
+    <t>Hệ thống mã hóa mẫu?</t>
+  </si>
+  <si>
+    <t>Ai là người duyệt cho các hành động xóa, sửa?</t>
+  </si>
+  <si>
+    <t>Mỗi phòng ban có bao nhiêu loại user?</t>
   </si>
 </sst>
 </file>
@@ -183,26 +209,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -213,6 +244,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -261,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,7 +330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -507,175 +541,191 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" customWidth="1"/>
-    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="D14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="C18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>